<commit_message>
sum and not mean
</commit_message>
<xml_diff>
--- a/UNICEF_framework_V09.xlsx
+++ b/UNICEF_framework_V09.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/src/unicef-assessment-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEF13F5-E7C7-6B4F-8E78-9901A38D2F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6279305-4BA7-7F40-A647-149807E4ACDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26600" firstSheet="8" activeTab="24" xr2:uid="{3FD09917-E6D0-0445-86B2-2BC0BB705E34}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26600" firstSheet="8" activeTab="24" xr2:uid="{3FD09917-E6D0-0445-86B2-2BC0BB705E34}"/>
   </bookViews>
   <sheets>
     <sheet name="how to use the tool" sheetId="22" r:id="rId1"/>
@@ -5771,7 +5771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E070C3D3-4DAD-8F4C-97F3-0D0E4D227814}" type="CELLRANGE">
+                    <a:fld id="{707DA047-B014-7042-93F2-3D2315B8AA98}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5961,7 +5961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C1BBB58-273D-B448-B9A4-CA4025DE2D93}" type="CELLRANGE">
+                    <a:fld id="{B1B30E49-CF6D-5047-8B0C-1EF9507FE511}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -30075,7 +30075,7 @@
   <dimension ref="A1:AD78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37096,12 +37096,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="13">
-    <mergeCell ref="G135:H135"/>
-    <mergeCell ref="I135:J135"/>
-    <mergeCell ref="H102:J102"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="F121:H121"/>
     <mergeCell ref="K121:L121"/>
     <mergeCell ref="M121:O121"/>
     <mergeCell ref="K87:L87"/>
@@ -37109,6 +37103,12 @@
     <mergeCell ref="F102:G102"/>
     <mergeCell ref="F87:H87"/>
     <mergeCell ref="D101:J101"/>
+    <mergeCell ref="G135:H135"/>
+    <mergeCell ref="I135:J135"/>
+    <mergeCell ref="H102:J102"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="F121:H121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>